<commit_message>
:fire: Adding a lot of stuff
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/notthefinalproject/Competitions Participations.xlsx
+++ b/src/main/java/com/example/notthefinalproject/Competitions Participations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24703"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\KFUPM Faculty\211\SWE206\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nawafo/IdeaProjects/NotTheFinalProject/src/main/java/com/example/notthefinalproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{5385D188-FC28-48BC-B469-1B2004474D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95D0870D-6BFC-437B-94D9-BE3C0EE1B856}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4A7490-6455-9241-A481-D82079EBFA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{54FEB0A3-0501-489B-8C15-4473C17019CE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{54FEB0A3-0501-489B-8C15-4473C17019CE}"/>
   </bookViews>
   <sheets>
     <sheet name="STC &amp; Nokia" sheetId="1" r:id="rId1"/>
     <sheet name="CyberHub" sheetId="4" r:id="rId2"/>
+    <sheet name="Hey" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Competition Name</t>
   </si>
@@ -122,13 +123,19 @@
   </si>
   <si>
     <t>Faris Ahmad</t>
+  </si>
+  <si>
+    <t>NawafComp</t>
+  </si>
+  <si>
+    <t>Nawaf Alomari</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,17 +500,17 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -519,7 +526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -527,7 +534,7 @@
         <v>44481</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -548,7 +555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -571,7 +578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -594,7 +601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -617,7 +624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -650,19 +657,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51007B-8ACE-4628-8795-6036C126B75A}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -670,7 +677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -678,7 +685,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -686,7 +693,7 @@
         <v>44471</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -701,7 +708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -718,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -735,7 +742,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -752,7 +759,135 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>222256700</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A53AF4-5A15-BD4D-B260-3FD415F2C996}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>222253860</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>222256560</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>222279260</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -952,12 +1087,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -966,14 +1095,44 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9006B6A5-E967-4BEF-8719-FC1A3A1130F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9006B6A5-E967-4BEF-8719-FC1A3A1130F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a97023e5-11bd-43d5-b639-e24feb137d68"/>
+    <ds:schemaRef ds:uri="1de9efba-49b8-4d57-bca1-024618aa2d5a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C77F59-3AFA-4DAC-A2AB-5008718B0584}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3D51158-FE10-4504-8B91-E9E61FC99E70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3D51158-FE10-4504-8B91-E9E61FC99E70}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C77F59-3AFA-4DAC-A2AB-5008718B0584}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>